<commit_message>
Avoid id conflicts when setting up a repository.
Actually this should be done by the constructor section in
general, but for now I add this fix to the
PathFromReferenceNumberSection which generates the path and id for all repositories.
</commit_message>
<xml_diff>
--- a/opengever/setup/tests/profiles/repositories/opengever_repositories/repo.xlsx
+++ b/opengever/setup/tests/profiles/repositories/opengever_repositories/repo.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28502"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flipsi/projects/opengever/koeniz/opengever/setup/tests/profiles/repositories/opengever_repositories/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ordnungssystem" sheetId="1" r:id="rId1"/>
@@ -14,6 +19,9 @@
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -57,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>reference_number</t>
   </si>
@@ -204,6 +212,12 @@
   </si>
   <si>
     <t>New Repository</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1.1</t>
   </si>
 </sst>
 </file>
@@ -414,6 +428,18 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -422,9 +448,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -449,26 +472,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -478,10 +492,15 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -815,10 +834,10 @@
   <dimension ref="A1:V47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.33203125" customWidth="1"/>
@@ -844,7 +863,7 @@
     <col min="24" max="24" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="5" customFormat="1">
+    <row r="1" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -857,7 +876,7 @@
       <c r="U1" s="7"/>
       <c r="V1"/>
     </row>
-    <row r="2" spans="1:22" s="5" customFormat="1">
+    <row r="2" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -869,80 +888,80 @@
       <c r="U2" s="7"/>
       <c r="V2"/>
     </row>
-    <row r="3" spans="1:22" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="24"/>
-      <c r="B3" s="26" t="s">
+    <row r="3" spans="1:22" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="27"/>
+      <c r="B3" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="22" t="s">
         <v>31</v>
       </c>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="11"/>
-      <c r="Q3" s="32" t="s">
+      <c r="Q3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="R3" s="32" t="s">
+      <c r="R3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="S3" s="32" t="s">
+      <c r="S3" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="T3" s="32" t="s">
+      <c r="T3" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="U3" s="32" t="s">
+      <c r="U3" s="20" t="s">
         <v>36</v>
       </c>
       <c r="V3"/>
     </row>
-    <row r="4" spans="1:22" s="5" customFormat="1" ht="77.25" customHeight="1">
-      <c r="A4" s="25"/>
-      <c r="B4" s="27"/>
+    <row r="4" spans="1:22" s="5" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="28"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="26"/>
       <c r="J4" s="23"/>
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
-      <c r="M4" s="34"/>
+      <c r="M4" s="24"/>
       <c r="N4" s="13" t="s">
         <v>39</v>
       </c>
@@ -952,14 +971,14 @@
       <c r="P4" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
       <c r="V4"/>
     </row>
-    <row r="5" spans="1:22" ht="20" hidden="1" customHeight="1">
+    <row r="5" spans="1:22" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1040,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" t="s">
         <v>48</v>
@@ -1044,7 +1063,7 @@
         <v>51440</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>42</v>
       </c>
@@ -1076,217 +1095,227 @@
         <v>51440</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="14"/>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
       <c r="F8" s="18"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="14"/>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
       <c r="F9" s="18"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="14"/>
       <c r="F10" s="18"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="F11" s="18"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
       <c r="F13" s="18"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
       <c r="F14" s="18"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="F15" s="18"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="F16" s="18"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="F17" s="18"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="F18" s="18"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
       <c r="F20" s="18"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
       <c r="F21" s="18"/>
       <c r="K21" s="19"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="F22" s="18"/>
       <c r="K22" s="19"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="F23" s="18"/>
       <c r="K23" s="19"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="F24" s="18"/>
       <c r="K24" s="19"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="14"/>
       <c r="F25" s="18"/>
       <c r="K25" s="19"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
       <c r="F26" s="18"/>
       <c r="K26" s="19"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
       <c r="F27" s="18"/>
       <c r="K27" s="19"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
       <c r="F28" s="18"/>
       <c r="K28" s="19"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="14"/>
       <c r="F29" s="18"/>
       <c r="K29" s="19"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="14"/>
       <c r="F30" s="18"/>
       <c r="K30" s="19"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="14"/>
       <c r="F31" s="18"/>
       <c r="K31" s="19"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="14"/>
       <c r="F32" s="18"/>
       <c r="K32" s="19"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="14"/>
       <c r="F33" s="18"/>
       <c r="K33" s="19"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="14"/>
       <c r="F34" s="18"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="F35" s="18"/>
       <c r="K35" s="19"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="14"/>
       <c r="F36" s="18"/>
       <c r="K36" s="19"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="14"/>
       <c r="F37" s="18"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="14"/>
       <c r="K38" s="19"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="14"/>
       <c r="K39" s="19"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="14"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="14"/>
       <c r="F41" s="18"/>
       <c r="G41" s="19"/>
@@ -1294,21 +1323,21 @@
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="14"/>
       <c r="F42" s="18"/>
       <c r="G42" s="19"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="14"/>
       <c r="F43" s="18"/>
       <c r="G43" s="19"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="14"/>
       <c r="F44" s="18"/>
       <c r="G44" s="19"/>
@@ -1316,7 +1345,7 @@
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="14"/>
       <c r="F45" s="18"/>
       <c r="G45" s="19"/>
@@ -1324,7 +1353,7 @@
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="14"/>
       <c r="F46" s="18"/>
       <c r="G46" s="19"/>
@@ -1332,7 +1361,7 @@
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="14"/>
       <c r="F47" s="18"/>
       <c r="G47" s="19"/>
@@ -1342,14 +1371,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="M3:M4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="J3:J4"/>
@@ -1359,13 +1380,16 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="M3:M4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Handle spaces inside groups ids during repository import correctly.
</commit_message>
<xml_diff>
--- a/opengever/setup/tests/profiles/repositories/opengever_repositories/repo.xlsx
+++ b/opengever/setup/tests/profiles/repositories/opengever_repositories/repo.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>reference_number</t>
   </si>
@@ -218,6 +218,15 @@
   </si>
   <si>
     <t>1.1</t>
+  </si>
+  <si>
+    <t>gever_users, gever eingangskorb</t>
+  </si>
+  <si>
+    <t>gever_users</t>
+  </si>
+  <si>
+    <t>gever_users, gever eingangskorb , administratoren</t>
   </si>
 </sst>
 </file>
@@ -428,49 +437,49 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -834,7 +843,7 @@
   <dimension ref="A1:V47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -889,79 +898,79 @@
       <c r="V2"/>
     </row>
     <row r="3" spans="1:22" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27"/>
-      <c r="B3" s="29" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="20" t="s">
         <v>31</v>
       </c>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="11"/>
-      <c r="Q3" s="20" t="s">
+      <c r="Q3" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="R3" s="20" t="s">
+      <c r="R3" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="S3" s="20" t="s">
+      <c r="S3" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="T3" s="20" t="s">
+      <c r="T3" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="U3" s="20" t="s">
+      <c r="U3" s="32" t="s">
         <v>36</v>
       </c>
       <c r="V3"/>
     </row>
     <row r="4" spans="1:22" s="5" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22"/>
       <c r="J4" s="23"/>
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
-      <c r="M4" s="24"/>
+      <c r="M4" s="34"/>
       <c r="N4" s="13" t="s">
         <v>39</v>
       </c>
@@ -971,11 +980,11 @@
       <c r="P4" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
       <c r="V4"/>
     </row>
     <row r="5" spans="1:22" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1062,6 +1071,21 @@
       <c r="O6" s="1">
         <v>51440</v>
       </c>
+      <c r="Q6" t="s">
+        <v>52</v>
+      </c>
+      <c r="R6" t="s">
+        <v>51</v>
+      </c>
+      <c r="S6" t="s">
+        <v>51</v>
+      </c>
+      <c r="T6" t="s">
+        <v>51</v>
+      </c>
+      <c r="U6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
@@ -1371,6 +1395,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="M3:M4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="J3:J4"/>
@@ -1380,14 +1412,6 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="M3:M4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>